<commit_message>
Added Due driver files
</commit_message>
<xml_diff>
--- a/RBV2/RBV2 Pin Assignments.xlsx
+++ b/RBV2/RBV2 Pin Assignments.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>DIO</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>59 (A5)</t>
+  </si>
+  <si>
+    <t>Servo</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>Wait button</t>
   </si>
 </sst>
 </file>
@@ -438,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,11 +550,17 @@
       <c r="A12">
         <v>12</v>
       </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -640,43 +655,59 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>23</v>
+      <c r="A27">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>12</v>
+      <c r="A28">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>27</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>